<commit_message>
Updated logistic and multinomial fits
</commit_message>
<xml_diff>
--- a/multinomial_logistic_fits/summary_table_growth_rates_effect on R_logistic multinomial models.xlsx
+++ b/multinomial_logistic_fits/summary_table_growth_rates_effect on R_logistic multinomial models.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="68">
   <si>
     <t>UK</t>
   </si>
@@ -123,30 +123,15 @@
     <t>Wales</t>
   </si>
   <si>
-    <t>VOC vs. B.1.177</t>
-  </si>
-  <si>
-    <t>VOC vs. minority variants</t>
-  </si>
-  <si>
-    <t>B.1.177 vs. minority variants</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
-    <t>VOC vs. all other  variants</t>
-  </si>
-  <si>
     <t>(1|LTLA/obs) + REGION * DATE</t>
   </si>
   <si>
     <t>3b</t>
   </si>
   <si>
-    <t>B.1.177 vs. all other variants</t>
-  </si>
-  <si>
     <t>DK+UK</t>
   </si>
   <si>
@@ -186,19 +171,10 @@
     <t>separate-slopes binomial GLMM</t>
   </si>
   <si>
-    <t>PS For model 1c the problem is that the delta_r you calculate completely depends on what timeframe one focuses on...</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
     <t>S2</t>
-  </si>
-  <si>
-    <t>B.1.1.7 vs. all other variants</t>
-  </si>
-  <si>
-    <t>B.1.1.7 vs. minority variants</t>
   </si>
   <si>
     <r>
@@ -265,6 +241,58 @@
     </r>
   </si>
   <si>
+    <t>(1|LTLA/OBS) + REGION + DATE</t>
+  </si>
+  <si>
+    <t>(1|LTLA/OBS) + REGION * DATE</t>
+  </si>
+  <si>
+    <t>(1|OBS) +  REGION + DATE</t>
+  </si>
+  <si>
+    <t>(1|OBS) +  REGION + COUNTRY*DATE</t>
+  </si>
+  <si>
+    <t>LTLA</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>PS2 if you like you can re-express M1 and M2 in terms of % increase in R value if that would look nicer ((M1-1) x 100 = % increase)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 1. Estimates of the selective advantage of the VOC 202012/01 in comparison to other SARS-CoV2 lineages, as measured by the selection rate </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>r (the slope on a log(odds) scale and also equal to the difference in Malthusian growth rates), as well as the implied multiplicative effect on the effective reproduction numbers Rt, assuming a generation time of either 5.5 or 3.6 days (M1 and M2), and assuming unaltered generation times. Some comparisons involving lineage B.1.177, which was the dominant lineage in the UK in much of the fall before VOC 202012/01 invaded, are also shown for comparison. The right hand side of the model formula's uses the notation as in the glmer function of R's lme4 package, with (1|) standing for random effect intercepts, / standing for nesting and * standing for main effects plus their interaction (factors REGION = NHS region, continuous covariate DATE = sampling date). Where possible, observation-level random effects (data-row index OBS) were included to take into account overdispersion.</t>
+    </r>
+  </si>
+  <si>
+    <t>PS1 For model 1c the delta_r one calculates heavily depends on what timeframe one focuses on, due to the time-varying selection rate we are allowing there...</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VOC vs. all other  variants </t>
+    </r>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
@@ -274,17 +302,95 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">a  </t>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VOC vs. B.1.177 </t>
     </r>
     <r>
       <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Natural cubic spline term with 2 degrees of freedom. </t>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VOC vs. minority variants </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B.1.177 vs. all other variants </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B.1.177 vs. minority variants </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <t>Table S1. Estimates of the selective advantage of the VOC 202012/01 and lineage B.1.1.7 in comparison to other SARS-CoV2 lineages across different PHE regions , as measured by the selection rate Dr (the slope on a log(odds) scale and also equal to the difference in Malthusian growth rates), as well as the implied multiplicative effect on the effective reproduction numbers Rt, assuming a generation time of either 5.5 or 3.6 days (M1 and M2), and assuming unaltered generation times. The right hand side of the model formula's uses the notation as in the glmer function of R's lme4 package, with (1|) standing for random effect intercepts, / standing for nesting and * standing for main effects plus their interaction (factors REGION = NHS region, continuous covariate DATE = sampling date). Where possible, observation-level random effects (data-row index OBS) were included to take into account overdispersion.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VOC vs. all other  variants </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B.1.1.7 vs. all other variants </t>
     </r>
     <r>
       <rPr>
@@ -297,19 +403,69 @@
       </rPr>
       <t>b</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B.1.1.7 vs. minority variants </t>
+    </r>
     <r>
       <rPr>
+        <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>b</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">a  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Natural cubic spline term with 2 degrees of freedom. </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">  Growth differences (</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Symbol"/>
         <family val="1"/>
@@ -319,7 +475,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -328,70 +484,107 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) in this model are time-dependent; for the VOC vs. minority variants and VOC vs. B.1.177 variant contrasts, growth differences were evaluated for the period from November 1 2020 until December 17 2020, when the VOC was invading and actively spreading, while for the B.1.177  vs. minority variants contrast, they are evaluated for the period from July 1st 2020 until the 30th of September 2020, when B.1.177 was invading.</t>
-    </r>
-  </si>
-  <si>
-    <t>(1|LTLA/OBS) + REGION + DATE</t>
-  </si>
-  <si>
-    <t>(1|LTLA/OBS) + REGION * DATE</t>
-  </si>
-  <si>
-    <t>(1|OBS) +  REGION + DATE</t>
-  </si>
-  <si>
-    <t>(1|OBS) +  REGION + COUNTRY*DATE</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Table 1. Estimates of the selective advantage of the VOC 202012/01 in comparison to other SARS-CoV2 lineages, as measured by the selection rate </t>
+      <t xml:space="preserve">) in this model are time-dependent; for the VOC vs. minority variants and VOC vs. B.1.177 variant contrasts, growth differences were evaluated for the period from November 1 2020 onwards and from July 1st 2020 until the 30th of September 2020, respectively, when each of these variants were actively invading in the population. </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>r (the slope on a log(odds) scale and also equal to the difference in Malthusian growth rate), as well as the implied multiplicative effect on the effective reproduction numbers Rt, assuming a generation time of either 5.5 or 3.6 days (M1 and M2), and assuming unaltered generation times. Some comparisons involving lineage B.1.177, which was the dominant lineage in the UK in much of the fall before VOC 202012/01 invaded, are also shown for comparison. The right hand side of the model formula's uses the notation as in the glmer function of R's lme4 package, with (1|) standing for random effect intercepts, / standing for nesting and * standing for main effects plus their interaction (factors REGION = NHS region, continuous covariate DATE = sampling date). Where possible, observation-level random effects (data-row index OBS) were included to take into account overdispersion.</t>
-    </r>
-  </si>
-  <si>
-    <t>PS if you like you can re-express M1 and M2 in terms of % increase in R value if that would look nicer ((M1-1) x 100 = % increase)</t>
-  </si>
-  <si>
-    <t>PHEREGION</t>
-  </si>
-  <si>
-    <t>LTLA</t>
-  </si>
-  <si>
-    <t>REGION</t>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Using a subset of the data from August 1 2020 onwards, omitting the zero counts in the earlier period. </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Using a subset of the data for the period between July 1st 2020 and September 30 2020, when the growth of this variant was approximately logistic, and before it started to be displaced by VOC 202012/01.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Using a subset of the data from August 1 2020 onwards, omitting the zero counts in the earlier period. </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Using a subset of the data for the period between July 1st 2020 and September 30 2020, when the growth of this variant was approximately logistic, and before it started to be displaced by VOC 202012/01 (Fig. S2).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,6 +751,34 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -744,7 +965,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -879,6 +1100,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -924,7 +1154,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,14 +1196,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1301,7 +1543,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A15" sqref="A15:Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,25 +1560,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="5" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I2" s="2"/>
@@ -1363,7 +1605,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>8</v>
@@ -1378,28 +1620,28 @@
         <v>5</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>2</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1413,19 +1655,19 @@
         <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="I4" s="1">
         <v>0.10496089432971401</v>
@@ -1458,7 +1700,7 @@
     <row r="5" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="G5" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="I5" s="1">
         <v>0.106738589985391</v>
@@ -1491,7 +1733,7 @@
     <row r="6" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="G6" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I6" s="1">
         <v>4.4870895868709897E-2</v>
@@ -1523,7 +1765,7 @@
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>0</v>
@@ -1532,19 +1774,19 @@
         <v>15</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="I7" s="1">
         <v>0.109301054651236</v>
@@ -1576,7 +1818,7 @@
     </row>
     <row r="8" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>0</v>
@@ -1585,19 +1827,19 @@
         <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="I8" s="1">
         <v>0.105953241732649</v>
@@ -1629,7 +1871,7 @@
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>0</v>
@@ -1638,19 +1880,19 @@
         <v>15</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="I9" s="1">
         <v>0.117332783333603</v>
@@ -1682,7 +1924,7 @@
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>0</v>
@@ -1691,19 +1933,19 @@
         <v>15</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="I10" s="1">
         <v>4.7557050240538502E-2</v>
@@ -1735,7 +1977,7 @@
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>0</v>
@@ -1744,19 +1986,19 @@
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="I11" s="1">
         <v>4.1916404873624101E-2</v>
@@ -1788,7 +2030,7 @@
     </row>
     <row r="12" spans="1:17" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>10</v>
@@ -1797,19 +2039,19 @@
         <v>15</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="I12" s="1">
         <v>9.5869078299830199E-2</v>
@@ -1841,28 +2083,28 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="I13" s="1">
         <v>8.3906437547806606E-2</v>
@@ -1902,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="6">
@@ -1933,54 +2175,54 @@
         <v>1.5255230670959401</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-    </row>
-    <row r="16" spans="1:17" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
+    <row r="15" spans="1:17" s="8" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:17" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:1" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2003,10 +2245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:R31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,6 +2266,28 @@
     <col min="19" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:18" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+    </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>9</v>
@@ -2041,7 +2305,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>13</v>
@@ -2080,9 +2344,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>0</v>
@@ -2091,10 +2355,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>0</v>
@@ -2103,10 +2367,10 @@
         <v>17</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="J4" s="1">
         <v>0.105634046981436</v>
@@ -2400,365 +2664,722 @@
         <v>1.6183550321798299</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="18" t="s">
+      <c r="D13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="20" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+      <c r="I13" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="21">
+        <v>4.9977772397893298E-2</v>
+      </c>
+      <c r="K13" s="21">
+        <v>3.9365757034201102E-2</v>
+      </c>
+      <c r="L13" s="21">
+        <v>6.0589787761585599E-2</v>
+      </c>
+      <c r="M13" s="21">
+        <v>1.31636973644532</v>
+      </c>
+      <c r="N13" s="21">
+        <v>1.2417375685090699</v>
+      </c>
+      <c r="O13" s="21">
+        <v>1.39548752246393</v>
+      </c>
+      <c r="P13" s="21">
+        <v>1.1971215663784001</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>1.15225019899894</v>
+      </c>
+      <c r="R13" s="21">
+        <v>1.24374033168606</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+      <c r="J14" s="21">
+        <v>2.8914235415662001E-2</v>
+      </c>
+      <c r="K14" s="21">
+        <v>1.9487327223790901E-2</v>
+      </c>
+      <c r="L14" s="21">
+        <v>3.8341143607533101E-2</v>
+      </c>
+      <c r="M14" s="21">
+        <v>1.17237111820149</v>
+      </c>
+      <c r="N14" s="21">
+        <v>1.1131349343165799</v>
+      </c>
+      <c r="O14" s="21">
+        <v>1.23475959330742</v>
+      </c>
+      <c r="P14" s="21">
+        <v>1.10970170779855</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>1.07267376570925</v>
+      </c>
+      <c r="R14" s="21">
+        <v>1.1480078283417201</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="J15" s="21">
+        <v>3.5008295044711098E-2</v>
+      </c>
+      <c r="K15" s="21">
+        <v>2.4780036949636399E-2</v>
+      </c>
+      <c r="L15" s="21">
+        <v>4.52365531397858E-2</v>
+      </c>
+      <c r="M15" s="21">
+        <v>1.2123318123519999</v>
+      </c>
+      <c r="N15" s="21">
+        <v>1.14601442242105</v>
+      </c>
+      <c r="O15" s="21">
+        <v>1.2824868470116899</v>
+      </c>
+      <c r="P15" s="21">
+        <v>1.13431604090546</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>1.0933081861804199</v>
+      </c>
+      <c r="R15" s="21">
+        <v>1.17686202016886</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+      <c r="J16" s="21">
+        <v>4.0914722311825899E-2</v>
+      </c>
+      <c r="K16" s="21">
+        <v>2.7593449971702301E-2</v>
+      </c>
+      <c r="L16" s="21">
+        <v>5.4235994651949497E-2</v>
+      </c>
+      <c r="M16" s="21">
+        <v>1.2523615046271801</v>
+      </c>
+      <c r="N16" s="21">
+        <v>1.1638854977550199</v>
+      </c>
+      <c r="O16" s="21">
+        <v>1.3475632622773599</v>
+      </c>
+      <c r="P16" s="21">
+        <v>1.15869341084141</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>1.1044377919161099</v>
+      </c>
+      <c r="R16" s="21">
+        <v>1.21561434256794</v>
+      </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="J17" s="21">
+        <v>5.8286167093708402E-2</v>
+      </c>
+      <c r="K17" s="21">
+        <v>4.8402142811245601E-2</v>
+      </c>
+      <c r="L17" s="21">
+        <v>6.8170191376171196E-2</v>
+      </c>
+      <c r="M17" s="21">
+        <v>1.3779183509912001</v>
+      </c>
+      <c r="N17" s="21">
+        <v>1.30501141186669</v>
+      </c>
+      <c r="O17" s="21">
+        <v>1.45489837462989</v>
+      </c>
+      <c r="P17" s="21">
+        <v>1.2334686011021601</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>1.19035039590346</v>
+      </c>
+      <c r="R17" s="21">
+        <v>1.27814868222072</v>
+      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="J18" s="21">
+        <v>5.3695414711148498E-2</v>
+      </c>
+      <c r="K18" s="21">
+        <v>4.5078404277140903E-2</v>
+      </c>
+      <c r="L18" s="21">
+        <v>6.2312425145156197E-2</v>
+      </c>
+      <c r="M18" s="21">
+        <v>1.3435626513349901</v>
+      </c>
+      <c r="N18" s="21">
+        <v>1.28137180092682</v>
+      </c>
+      <c r="O18" s="21">
+        <v>1.40877190894683</v>
+      </c>
+      <c r="P18" s="21">
+        <v>1.2132509507721601</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>1.17619218106475</v>
+      </c>
+      <c r="R18" s="21">
+        <v>1.25147734634407</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="J19" s="21">
+        <v>3.5475546233032201E-2</v>
+      </c>
+      <c r="K19" s="21">
+        <v>2.83473986442664E-2</v>
+      </c>
+      <c r="L19" s="21">
+        <v>4.2603693821798003E-2</v>
+      </c>
+      <c r="M19" s="21">
+        <v>1.2154513682194299</v>
+      </c>
+      <c r="N19" s="21">
+        <v>1.16872182285558</v>
+      </c>
+      <c r="O19" s="21">
+        <v>1.2640493226154501</v>
+      </c>
+      <c r="P19" s="21">
+        <v>1.1362256844299199</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>1.10743954564184</v>
+      </c>
+      <c r="R19" s="21">
+        <v>1.1657600733500999</v>
+      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20" t="s">
         <v>24</v>
       </c>
+      <c r="J20" s="21">
+        <v>7.1434312855701398E-2</v>
+      </c>
+      <c r="K20" s="21">
+        <v>6.1638174611762402E-2</v>
+      </c>
+      <c r="L20" s="21">
+        <v>8.1230451099640499E-2</v>
+      </c>
+      <c r="M20" s="21">
+        <v>1.4812535473092301</v>
+      </c>
+      <c r="N20" s="21">
+        <v>1.4035573250859299</v>
+      </c>
+      <c r="O20" s="21">
+        <v>1.5632507715934301</v>
+      </c>
+      <c r="P20" s="21">
+        <v>1.2932565909089899</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>1.2484433167208</v>
+      </c>
+      <c r="R20" s="21">
+        <v>1.3396784519801901</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="J21" s="21">
+        <v>4.1703825128324497E-2</v>
+      </c>
+      <c r="K21" s="21">
+        <v>3.3023002820991597E-2</v>
+      </c>
+      <c r="L21" s="21">
+        <v>5.0384647435657501E-2</v>
+      </c>
+      <c r="M21" s="21">
+        <v>1.25780864750349</v>
+      </c>
+      <c r="N21" s="21">
+        <v>1.19916624024809</v>
+      </c>
+      <c r="O21" s="21">
+        <v>1.3193188238915501</v>
+      </c>
+      <c r="P21" s="21">
+        <v>1.1619896722273699</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>1.12623792690703</v>
+      </c>
+      <c r="R21" s="21">
+        <v>1.1988763351906899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="18" t="s">
+      <c r="E22" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
+      <c r="H22" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="21">
+        <v>4.9549553876980498E-2</v>
+      </c>
+      <c r="K22" s="21">
+        <v>3.8935645463369098E-2</v>
+      </c>
+      <c r="L22" s="21">
+        <v>6.0163462290591899E-2</v>
+      </c>
+      <c r="M22" s="21">
+        <v>1.31327306805799</v>
+      </c>
+      <c r="N22" s="21">
+        <v>1.23880356890323</v>
+      </c>
+      <c r="O22" s="21">
+        <v>1.39221923037677</v>
+      </c>
+      <c r="P22" s="21">
+        <v>1.1952775214657001</v>
+      </c>
+      <c r="Q22" s="21">
+        <v>1.15046743345859</v>
+      </c>
+      <c r="R22" s="21">
+        <v>1.24183293830944</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18" t="s">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
+      <c r="J23" s="21">
+        <v>2.6727494627388899E-2</v>
+      </c>
+      <c r="K23" s="21">
+        <v>1.72288568930156E-2</v>
+      </c>
+      <c r="L23" s="21">
+        <v>3.6226132361762101E-2</v>
+      </c>
+      <c r="M23" s="21">
+        <v>1.15835537674455</v>
+      </c>
+      <c r="N23" s="21">
+        <v>1.0993935536509001</v>
+      </c>
+      <c r="O23" s="21">
+        <v>1.2204793946418599</v>
+      </c>
+      <c r="P23" s="21">
+        <v>1.1010001353327901</v>
+      </c>
+      <c r="Q23" s="21">
+        <v>1.06398775757514</v>
+      </c>
+      <c r="R23" s="21">
+        <v>1.1393000430432201</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
+      <c r="J24" s="21">
+        <v>3.2333680876867402E-2</v>
+      </c>
+      <c r="K24" s="21">
+        <v>2.2177556291251E-2</v>
+      </c>
+      <c r="L24" s="21">
+        <v>4.2489805462483703E-2</v>
+      </c>
+      <c r="M24" s="21">
+        <v>1.1946284837926799</v>
+      </c>
+      <c r="N24" s="21">
+        <v>1.1297276202047699</v>
+      </c>
+      <c r="O24" s="21">
+        <v>1.26325778777554</v>
+      </c>
+      <c r="P24" s="21">
+        <v>1.1234465659406001</v>
+      </c>
+      <c r="Q24" s="21">
+        <v>1.08311289198744</v>
+      </c>
+      <c r="R24" s="21">
+        <v>1.1652822119103501</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
+      <c r="J25" s="21">
+        <v>4.1430814057035699E-2</v>
+      </c>
+      <c r="K25" s="21">
+        <v>2.7798453104250199E-2</v>
+      </c>
+      <c r="L25" s="21">
+        <v>5.5063175009821101E-2</v>
+      </c>
+      <c r="M25" s="21">
+        <v>1.2559213885004199</v>
+      </c>
+      <c r="N25" s="21">
+        <v>1.16519853880543</v>
+      </c>
+      <c r="O25" s="21">
+        <v>1.35370795753822</v>
+      </c>
+      <c r="P25" s="21">
+        <v>1.1608481835066899</v>
+      </c>
+      <c r="Q25" s="21">
+        <v>1.1052531803073899</v>
+      </c>
+      <c r="R25" s="21">
+        <v>1.2192396540094199</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
+      <c r="J26" s="21">
+        <v>5.5139528466793999E-2</v>
+      </c>
+      <c r="K26" s="21">
+        <v>4.5015582433274498E-2</v>
+      </c>
+      <c r="L26" s="21">
+        <v>6.5263474500313404E-2</v>
+      </c>
+      <c r="M26" s="21">
+        <v>1.3542765584727401</v>
+      </c>
+      <c r="N26" s="21">
+        <v>1.28092913764009</v>
+      </c>
+      <c r="O26" s="21">
+        <v>1.43182393384206</v>
+      </c>
+      <c r="P26" s="21">
+        <v>1.2195748354582401</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>1.17592620512066</v>
+      </c>
+      <c r="R26" s="21">
+        <v>1.26484363798185</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
+      <c r="J27" s="21">
+        <v>5.1613402775062503E-2</v>
+      </c>
+      <c r="K27" s="21">
+        <v>4.2788435138237602E-2</v>
+      </c>
+      <c r="L27" s="21">
+        <v>6.0438370411887397E-2</v>
+      </c>
+      <c r="M27" s="21">
+        <v>1.3282651805416701</v>
+      </c>
+      <c r="N27" s="21">
+        <v>1.26533434709443</v>
+      </c>
+      <c r="O27" s="21">
+        <v>1.3943258506265299</v>
+      </c>
+      <c r="P27" s="21">
+        <v>1.2041913345381501</v>
+      </c>
+      <c r="Q27" s="21">
+        <v>1.16653564180685</v>
+      </c>
+      <c r="R27" s="21">
+        <v>1.24306255051988</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
+      <c r="J28" s="21">
+        <v>1.7046291214176699E-2</v>
+      </c>
+      <c r="K28" s="21">
+        <v>9.0750044235422406E-3</v>
+      </c>
+      <c r="L28" s="21">
+        <v>2.5017578004811102E-2</v>
+      </c>
+      <c r="M28" s="21">
+        <v>1.09829019427399</v>
+      </c>
+      <c r="N28" s="21">
+        <v>1.05117913975401</v>
+      </c>
+      <c r="O28" s="21">
+        <v>1.1475126410144201</v>
+      </c>
+      <c r="P28" s="21">
+        <v>1.0632886957946901</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>1.0332095402876</v>
+      </c>
+      <c r="R28" s="21">
+        <v>1.09424352613901</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18" t="s">
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
+      <c r="J29" s="21">
+        <v>6.7881800656802604E-2</v>
+      </c>
+      <c r="K29" s="21">
+        <v>5.79674559676506E-2</v>
+      </c>
+      <c r="L29" s="21">
+        <v>7.7796145345954706E-2</v>
+      </c>
+      <c r="M29" s="21">
+        <v>1.4525925182903701</v>
+      </c>
+      <c r="N29" s="21">
+        <v>1.3755050982171</v>
+      </c>
+      <c r="O29" s="21">
+        <v>1.5340001479661001</v>
+      </c>
+      <c r="P29" s="21">
+        <v>1.2768223884387899</v>
+      </c>
+      <c r="Q29" s="21">
+        <v>1.2320541800818801</v>
+      </c>
+      <c r="R29" s="21">
+        <v>1.3232173048673801</v>
+      </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24">
+        <v>3.5525077307356101E-2</v>
+      </c>
+      <c r="K30" s="24">
+        <v>2.6884859550473102E-2</v>
+      </c>
+      <c r="L30" s="24">
+        <v>4.41652950642391E-2</v>
+      </c>
+      <c r="M30" s="24">
+        <v>1.2157825276910701</v>
+      </c>
+      <c r="N30" s="24">
+        <v>1.1593583755094199</v>
+      </c>
+      <c r="O30" s="24">
+        <v>1.2749527547850901</v>
+      </c>
+      <c r="P30" s="24">
+        <v>1.13642830501798</v>
+      </c>
+      <c r="Q30" s="24">
+        <v>1.1016240437282401</v>
+      </c>
+      <c r="R30" s="24">
+        <v>1.1723321579613399</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A31:R31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>